<commit_message>
se crea el programa copiar_info_reunion
</commit_message>
<xml_diff>
--- a/Info_Reuniones_Backup.xlsx
+++ b/Info_Reuniones_Backup.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cf898251a53e4db5/JW/Asignaciones Congregación/Ancianos/Super VMC/Programación-VMC/2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_085D688751585A0E6235547658BD3EFBA86D8A9F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81B018BA-80EA-45E7-BE90-FF85D0258D4E}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_085D3457D054720F6235547658BD3EFBA86D8A9F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC9F4317-5B3D-45A3-8AE7-190E5D8AEA44}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Info-reunión" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -146,7 +146,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -494,7 +493,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>